<commit_message>
Can decide on match from (first) sheet. runs smoothly
</commit_message>
<xml_diff>
--- a/Karim/strings stems.xlsx
+++ b/Karim/strings stems.xlsx
@@ -1365,21 +1365,21 @@
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="24.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="13.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2518,7 +2518,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.06"/>
@@ -3184,7 +3184,7 @@
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3643,7 +3643,7 @@
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4391,7 +4391,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4414,7 +4414,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4458,7 +4458,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4547,7 +4547,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4581,7 +4581,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
Added scripts. Followed the correct steps of operation. code now checks against already_sent
</commit_message>
<xml_diff>
--- a/Karim/strings stems.xlsx
+++ b/Karim/strings stems.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" state="visible" r:id="rId2"/>
@@ -870,7 +870,7 @@
     <t xml:space="preserve">davinc</t>
   </si>
   <si>
-    <t xml:space="preserve">x</t>
+    <t xml:space="preserve">karim</t>
   </si>
   <si>
     <t xml:space="preserve">name</t>
@@ -1249,7 +1249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1279,6 +1279,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1329,7 +1335,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1339,6 +1345,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1361,14 +1371,14 @@
   </sheetPr>
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A54" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C99" activeCellId="0" sqref="C99"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.64"/>
@@ -2512,11 +2522,11 @@
   </sheetPr>
   <dimension ref="A1:DF35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AQ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BB1" activeCellId="0" sqref="BB1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.44"/>
@@ -3335,61 +3345,61 @@
       <c r="B15" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="L15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="M15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="S15" s="2" t="s">
+      <c r="S15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="AC15" s="2" t="s">
+      <c r="AC15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="AE15" s="2" t="s">
+      <c r="AE15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="AH15" s="2" t="s">
+      <c r="AH15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="BI15" s="2" t="s">
+      <c r="BI15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="BK15" s="2" t="s">
+      <c r="BK15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="BP15" s="2" t="s">
+      <c r="BP15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="BW15" s="2" t="s">
+      <c r="BW15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="CW15" s="2" t="s">
+      <c r="CW15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="DB15" s="2" t="s">
+      <c r="DB15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="DC15" s="2" t="s">
+      <c r="DC15" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="DD15" s="2" t="s">
+      <c r="DD15" s="3" t="s">
         <v>280</v>
       </c>
     </row>
@@ -3416,11 +3426,11 @@
   </sheetPr>
   <dimension ref="A1:A90"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -3875,11 +3885,11 @@
   </sheetPr>
   <dimension ref="A1:A111"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B91" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4458,7 +4468,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4481,7 +4491,7 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4531,7 +4541,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4620,7 +4630,7 @@
       <selection pane="topLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4660,7 +4670,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">

</xml_diff>

<commit_message>
fixed bugs for messed up all_info table. Added clear data functionality
</commit_message>
<xml_diff>
--- a/Karim/strings stems.xlsx
+++ b/Karim/strings stems.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="first" sheetId="1" state="visible" r:id="rId2"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="404">
   <si>
     <t xml:space="preserve">a graphic designer</t>
   </si>
@@ -495,6 +495,9 @@
     <t xml:space="preserve">drupal </t>
   </si>
   <si>
+    <t xml:space="preserve">graphic</t>
+  </si>
+  <si>
     <t xml:space="preserve">salesforce</t>
   </si>
   <si>
@@ -1120,9 +1123,6 @@
   </si>
   <si>
     <t xml:space="preserve">no money</t>
-  </si>
-  <si>
-    <t xml:space="preserve">graphic</t>
   </si>
   <si>
     <t xml:space="preserve">video </t>
@@ -1249,7 +1249,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1279,12 +1279,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1335,7 +1329,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1345,10 +1339,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1371,11 +1361,11 @@
   </sheetPr>
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.59"/>
@@ -2105,403 +2095,406 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>155</v>
+      </c>
       <c r="C31" s="0" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C32" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C34" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C35" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C36" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C38" s="0" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C41" s="0" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C42" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C43" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="0" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C53" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C54" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C55" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C56" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C58" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C59" s="0" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C60" s="0" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C61" s="0" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C62" s="0" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C63" s="0" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C64" s="0" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C65" s="0" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C66" s="0" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="0" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C68" s="0" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C69" s="0" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C70" s="0" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C71" s="0" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C72" s="0" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C73" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C74" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C75" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C76" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C77" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C78" s="0" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C79" s="0" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C80" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C81" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C82" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C83" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C84" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C85" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C86" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C87" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C88" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C89" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C90" s="0" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C91" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C92" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C93" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C94" s="0" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C95" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C96" s="0" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C97" s="0" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C98" s="1" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C99" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C100" s="0" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C101" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C102" s="0" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C103" s="0" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C104" s="0" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C105" s="0" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C106" s="0" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C107" s="0" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C108" s="0" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C109" s="0" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C110" s="0" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -2522,11 +2515,11 @@
   </sheetPr>
   <dimension ref="A1:DF35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.44"/>
@@ -2543,7 +2536,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="16.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="16.94"/>
-    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="26" min="26" style="0" width="8.67"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="26" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="0" width="13.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="18.89"/>
@@ -2559,70 +2552,70 @@
         <v>153</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>69</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="V1" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="W1" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>35</v>
@@ -2637,16 +2630,16 @@
         <v>46</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AF1" s="1" t="s">
         <v>77</v>
@@ -2664,58 +2657,58 @@
         <v>154</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AW1" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AX1" s="1" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="AY1" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="BA1" s="1" t="s">
         <v>132</v>
       </c>
       <c r="BB1" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="BC1" s="1" t="s">
         <v>121</v>
@@ -2727,7 +2720,7 @@
         <v>14</v>
       </c>
       <c r="BF1" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BG1" s="1" t="s">
         <v>76</v>
@@ -2760,25 +2753,25 @@
         <v>61</v>
       </c>
       <c r="BQ1" s="1" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="BR1" s="1" t="s">
         <v>67</v>
       </c>
       <c r="BS1" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="BT1" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="BU1" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="BV1" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="BW1" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="BX1" s="1" t="s">
         <v>26</v>
@@ -2847,40 +2840,40 @@
         <v>134</v>
       </c>
       <c r="CT1" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CU1" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="CV1" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="CW1" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="CX1" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="CY1" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="CZ1" s="1" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="DA1" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="DB1" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="DC1" s="1" t="s">
         <v>88</v>
       </c>
       <c r="DD1" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="DE1" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2900,7 +2893,7 @@
         <v>15</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>56</v>
@@ -2909,13 +2902,13 @@
         <v>75</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="L2" s="0" t="s">
         <v>13</v>
@@ -2924,31 +2917,31 @@
         <v>98</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="U2" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="V2" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="V2" s="0" t="s">
-        <v>176</v>
-      </c>
       <c r="W2" s="0" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="X2" s="0" t="s">
         <v>48</v>
@@ -2966,13 +2959,13 @@
         <v>72</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="AG2" s="0" t="s">
         <v>136</v>
@@ -2987,70 +2980,70 @@
         <v>154</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AM2" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="AN2" s="0" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="AO2" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="AP2" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="AQ2" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="AS2" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="AT2" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="AU2" s="0" t="s">
         <v>42</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="AW2" s="1" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="AX2" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="AY2" s="0" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="BA2" s="1" t="s">
         <v>132</v>
       </c>
       <c r="BB2" s="1" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="BC2" s="1" t="s">
         <v>121</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="BG2" s="1" t="s">
         <v>76</v>
@@ -3083,7 +3076,7 @@
         <v>61</v>
       </c>
       <c r="BQ2" s="0" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="BR2" s="1" t="s">
         <v>67</v>
@@ -3092,13 +3085,13 @@
         <v>133</v>
       </c>
       <c r="BU2" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="BV2" s="1" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="BW2" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="BX2" s="1" t="s">
         <v>26</v>
@@ -3167,7 +3160,7 @@
         <v>134</v>
       </c>
       <c r="CT2" s="1" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="CU2" s="1" t="s">
         <v>127</v>
@@ -3176,13 +3169,13 @@
         <v>141</v>
       </c>
       <c r="CW2" s="0" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="CX2" s="1" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="CY2" s="1" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="CZ2" s="1" t="s">
         <v>135</v>
@@ -3191,16 +3184,16 @@
         <v>103</v>
       </c>
       <c r="DB2" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="DC2" s="0" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="DD2" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="DE2" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="DF2" s="1"/>
     </row>
@@ -3209,13 +3202,13 @@
         <v>43</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>131</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>22</v>
@@ -3224,31 +3217,31 @@
         <v>147</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="AN3" s="0" t="s">
         <v>149</v>
       </c>
       <c r="AY3" s="1" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="BD3" s="1" t="s">
         <v>71</v>
@@ -3258,7 +3251,7 @@
       </c>
       <c r="BW3" s="1"/>
       <c r="DE3" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3269,22 +3262,22 @@
         <v>116</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F4" s="0" t="s">
         <v>63</v>
       </c>
       <c r="AC4" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="AN4" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="DE4" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3295,10 +3288,10 @@
         <v>25</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AC5" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3306,13 +3299,13 @@
         <v>36</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AC6" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3325,82 +3318,82 @@
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AC8" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AC9" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AC10" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="S15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="AC15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="AE15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="AH15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="BI15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="BK15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="BP15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="BW15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="CW15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="DB15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="DC15" s="3" t="s">
-        <v>280</v>
-      </c>
-      <c r="DD15" s="3" t="s">
-        <v>280</v>
+        <v>281</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="AC15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="AE15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="AH15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="BI15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="BK15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="BP15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="BW15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="CW15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="DB15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="DC15" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="DD15" s="2" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3430,441 +3423,441 @@
       <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
   </sheetData>
@@ -3889,11 +3882,11 @@
       <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3903,7 +3896,7 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>364</v>
+        <v>155</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3958,12 +3951,12 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3983,12 +3976,12 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4123,52 +4116,52 @@
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4178,7 +4171,7 @@
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4303,7 +4296,7 @@
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4318,7 +4311,7 @@
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4338,7 +4331,7 @@
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4378,12 +4371,12 @@
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4433,17 +4426,17 @@
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -4468,7 +4461,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4491,11 +4484,11 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4541,7 +4534,7 @@
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -4595,7 +4588,7 @@
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4630,11 +4623,11 @@
       <selection pane="topLeft" activeCell="M29" activeCellId="0" sqref="M29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4670,11 +4663,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>